<commit_message>
nota EV02 y sprint 2
</commit_message>
<xml_diff>
--- a/Equipo07/Fase 2/Evidencias_Proyecto/Evidencias_de_documentacion/Product_Backlog_Estimacion_Historias_DFF.xlsx
+++ b/Equipo07/Fase 2/Evidencias_Proyecto/Evidencias_de_documentacion/Product_Backlog_Estimacion_Historias_DFF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jotas\Desktop\Documentos Capstone (SCRUM)\backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jotas\Desktop\Capstone_Equipo07_Fase1\Equipo07\Fase 2\Evidencias_Proyecto\Evidencias_de_documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C8FABE-71F4-4847-A10E-6956A1CBF074}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DFB889-F57A-498A-A453-F0C04BD028BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product_Backlog" sheetId="1" r:id="rId1"/>
@@ -143,13 +143,13 @@
     <t>Como dueña de la florería necesito organizar productos por categorías para facilitar búsqueda y reportes.</t>
   </si>
   <si>
-    <t>Como cliente quiero recibir una boleta digital para tener comprobante de mi compra.</t>
-  </si>
-  <si>
-    <t>Como dueña de la florería necesito registrar ventas y generar boletas en PDF para entregar comprobantes a clientes.</t>
-  </si>
-  <si>
     <t>Como dueña de la florería necesito registrar compras a proveedores para mantener control y actualizar inventario automáticamente.</t>
+  </si>
+  <si>
+    <t>Como cliente quiero recibir un comprobante digital para tener constancia de mi compra.</t>
+  </si>
+  <si>
+    <t>Como dueña de la florería necesito registrar ventas y generar boletas para entregar comprobantes a clientes.</t>
   </si>
 </sst>
 </file>
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -735,7 +735,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C6" s="8">
         <v>8</v>
@@ -746,7 +746,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" s="8">
         <v>13</v>
@@ -757,7 +757,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="8">
         <v>3</v>

</xml_diff>